<commit_message>
Halfway in creating the 6par model
</commit_message>
<xml_diff>
--- a/matlab_examples.xlsx
+++ b/matlab_examples.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\Matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0E08B8-C91C-417A-ACB4-B180FCE1DB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE943987-017B-49FF-B77F-643A71CAC6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
-    <sheet name="n=10" sheetId="1" r:id="rId1"/>
-    <sheet name="n=8" sheetId="2" r:id="rId2"/>
-    <sheet name="VQ_n=8" sheetId="4" r:id="rId3"/>
+    <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
+    <sheet name="n=8,4par" sheetId="2" r:id="rId2"/>
+    <sheet name="n=8,6par" sheetId="5" r:id="rId3"/>
+    <sheet name="VQ_n=8,4par" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>A1</t>
   </si>
@@ -178,6 +179,18 @@
   </si>
   <si>
     <t>Ref_POC=24</t>
+  </si>
+  <si>
+    <t>SIX PARAMETER MODEL</t>
+  </si>
+  <si>
+    <t>ESEMPIO 7</t>
+  </si>
+  <si>
+    <t>Block (96,192)</t>
+  </si>
+  <si>
+    <t>Matlab è d'accordo con VQ Analyzer</t>
   </si>
 </sst>
 </file>
@@ -199,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +243,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -252,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -264,6 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -492,6 +512,61 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>169766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF88FAC6-C4F3-4379-A6C8-4E7325C07A7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3638550" y="931766"/>
+          <a:ext cx="5248275" cy="4183159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1224,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEB8DE-3B5F-446A-887E-6DEB4FE5A1BA}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,11 +1624,214 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28471F49-110A-464B-B794-649FAD3DFDB3}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>68</v>
+      </c>
+      <c r="D15">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>75</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>64</v>
+      </c>
+      <c r="D20">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>88</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>96</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65113F10-061B-4B09-B2DF-139F685758A8}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Six parameter model complete
</commit_message>
<xml_diff>
--- a/matlab_examples.xlsx
+++ b/matlab_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE943987-017B-49FF-B77F-643A71CAC6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740C927-7D77-439E-B5F2-53E9380A8BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
   <si>
     <t>A1</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Matlab è d'accordo con VQ Analyzer</t>
+  </si>
+  <si>
+    <t>Cur_POC =1</t>
+  </si>
+  <si>
+    <t>Ref_POC=0</t>
   </si>
 </sst>
 </file>
@@ -1627,11 +1633,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28471F49-110A-464B-B794-649FAD3DFDB3}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1680,10 +1689,15 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added an example from BasketballPass
</commit_message>
<xml_diff>
--- a/matlab_examples.xlsx
+++ b/matlab_examples.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740C927-7D77-439E-B5F2-53E9380A8BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D83C9-D218-4ABB-8ADE-4E707126E07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
+    <workbookView xWindow="-9210" yWindow="2265" windowWidth="15375" windowHeight="7875" activeTab="5" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
     <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
     <sheet name="n=8,4par" sheetId="2" r:id="rId2"/>
     <sheet name="n=8,6par" sheetId="5" r:id="rId3"/>
     <sheet name="VQ_n=8,4par" sheetId="4" r:id="rId4"/>
+    <sheet name="VQ_n=8,6par" sheetId="6" r:id="rId5"/>
+    <sheet name="Basket_n=8,6par" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="69">
   <si>
     <t>A1</t>
   </si>
@@ -197,6 +199,54 @@
   </si>
   <si>
     <t>Ref_POC=0</t>
+  </si>
+  <si>
+    <t>ESEMPIO 8</t>
+  </si>
+  <si>
+    <t>Cur_POC =12</t>
+  </si>
+  <si>
+    <t>Ref_POC=8</t>
+  </si>
+  <si>
+    <t>Size: 32x16</t>
+  </si>
+  <si>
+    <t>Block (160,128)</t>
+  </si>
+  <si>
+    <t>ESEMPIO 9</t>
+  </si>
+  <si>
+    <t>Block (208,96)</t>
+  </si>
+  <si>
+    <t>Cur_POC =34</t>
+  </si>
+  <si>
+    <t>Ref_POC=32</t>
+  </si>
+  <si>
+    <t>Seq: BasketballPass_416x240_50</t>
+  </si>
+  <si>
+    <t>File: BasketballPass_416x240_50.yuv</t>
+  </si>
+  <si>
+    <t>Coded YUV: BasketballPass_416x240_50_Coded_8bit.yuv</t>
+  </si>
+  <si>
+    <t>ESEMPIO 10</t>
+  </si>
+  <si>
+    <t>Block (224,104)</t>
+  </si>
+  <si>
+    <t>Cur_POC =49</t>
+  </si>
+  <si>
+    <t>Ref_POC=48</t>
   </si>
 </sst>
 </file>
@@ -677,6 +727,166 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{095A9A25-A10F-4B12-BBCE-942EDB5E97A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3838575" y="1166767"/>
+          <a:ext cx="5534025" cy="4414883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>61770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Immagine 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CB8D67A-F79C-4082-9CA6-15758FE00C58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3981450" y="6348270"/>
+          <a:ext cx="5410200" cy="4462605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F8033E-8D06-49B2-8E14-9D911C84FDF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="1381125"/>
+          <a:ext cx="6029325" cy="4238625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
@@ -1633,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28471F49-110A-464B-B794-649FAD3DFDB3}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65113F10-061B-4B09-B2DF-139F685758A8}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:D54"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,4 +2494,764 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DCD117-709F-4639-B4BF-045D3AB23B90}">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>127</v>
+      </c>
+      <c r="D15">
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>139</v>
+      </c>
+      <c r="D22">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>137</v>
+      </c>
+      <c r="D23">
+        <v>-127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>127</v>
+      </c>
+      <c r="D27">
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>64</v>
+      </c>
+      <c r="D29">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>137</v>
+      </c>
+      <c r="D31">
+        <v>-127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>-64</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>-80</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>-63</v>
+      </c>
+      <c r="D44">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>-91</v>
+      </c>
+      <c r="D46">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>-86</v>
+      </c>
+      <c r="D47">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>-34</v>
+      </c>
+      <c r="D49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>-64</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>-91</v>
+      </c>
+      <c r="D56">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>29</v>
+      </c>
+      <c r="D58">
+        <v>-24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451FC1BF-9EF4-43BD-A73C-08EC918EDEA4}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>59</v>
+      </c>
+      <c r="E22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>59</v>
+      </c>
+      <c r="E31">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>